<commit_message>
maj images _ ref  2024
</commit_message>
<xml_diff>
--- a/references/references_dsidd.xlsx
+++ b/references/references_dsidd.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSIDD2\d-sidd Dropbox\Equipe\sites internet\Site rmarkdown\site-dsidd\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AE9CDC-E320-430B-A1A5-6674321711BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A112414-29A0-4C73-B83E-C498C8BB7CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A1639DB-56E8-489A-8363-79F7F85173AB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A1639DB-56E8-489A-8363-79F7F85173AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="119">
   <si>
     <t>Développement économique durable des territoires</t>
   </si>
@@ -358,10 +361,43 @@
     <t>Tableaux de bord emploi formation Bâtiment et Travaux publics région Ile de France</t>
   </si>
   <si>
-    <t>2023 (en cours)</t>
-  </si>
-  <si>
-    <t>2022 (en cours)</t>
+    <t xml:space="preserve">Cartographie interactive pour l’accompagnement au diagnostic stratégique préalable d’un pacte local des solidarités dans le département de l’Allier </t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>2022, 2023, 2024</t>
+  </si>
+  <si>
+    <t>Observatoire de l' Immobilier d'Entreprise de Montpellier et son territoire Urbain</t>
+  </si>
+  <si>
+    <t>Observatoire de l'Immobilier du Commerce Montpellier et son territoire Urbain</t>
+  </si>
+  <si>
+    <t>DDETS du Var</t>
+  </si>
+  <si>
+    <t>Logi-cité</t>
+  </si>
+  <si>
+    <t>Terre d'Avance</t>
+  </si>
+  <si>
+    <t>CERC Ile de France</t>
+  </si>
+  <si>
+    <t>Département Allier</t>
+  </si>
+  <si>
+    <t>CERC Occitanie</t>
+  </si>
+  <si>
+    <t>Données de cadrage du plan départemental d'action pour le logement et l'hébergement des personnes défavorisées des Alpes de Hautes Provence</t>
+  </si>
+  <si>
+    <t>CEISS Consultants</t>
   </si>
 </sst>
 </file>
@@ -736,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B3B7FE-E50F-4A1F-B29E-52CC043F3381}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1865,6 +1901,12 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
       <c r="C39">
         <v>4</v>
       </c>
@@ -1885,6 +1927,12 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
       <c r="C40">
         <v>2</v>
       </c>
@@ -1894,8 +1942,8 @@
       <c r="E40" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F40" t="s">
-        <v>106</v>
+      <c r="F40">
+        <v>2023</v>
       </c>
       <c r="G40" s="1">
         <v>4400</v>
@@ -1905,6 +1953,12 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
       <c r="C41">
         <v>2</v>
       </c>
@@ -1925,6 +1979,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
       <c r="C42">
         <v>3</v>
       </c>
@@ -1935,7 +1995,7 @@
         <v>105</v>
       </c>
       <c r="F42">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G42" s="1">
         <v>13200</v>
@@ -1944,7 +2004,116 @@
         <v>55</v>
       </c>
     </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43">
+        <v>2023</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3400</v>
+      </c>
+      <c r="I43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="1">
+        <f>6300*2</f>
+        <v>12600</v>
+      </c>
+      <c r="I44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45">
+        <v>2022</v>
+      </c>
+      <c r="G45" s="1">
+        <v>6300</v>
+      </c>
+      <c r="I45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46">
+        <v>2022</v>
+      </c>
+      <c r="G46" s="1">
+        <v>3570</v>
+      </c>
+      <c r="I46" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J46" xr:uid="{D9B3B7FE-E50F-4A1F-B29E-52CC043F3381}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I38">
     <sortCondition ref="D2:D38"/>
     <sortCondition ref="F2:F38"/>

</xml_diff>